<commit_message>
small changes on laptop
</commit_message>
<xml_diff>
--- a/data/visit_dates.xlsx
+++ b/data/visit_dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucbtds4\R_Repositories\rodent_trapping\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/r_repositories/rodent_trapping/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0D3BE7-691B-46F8-88B8-8F441C40A711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F24920-CBB7-9246-904C-35D9A0395EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -383,15 +383,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -422,7 +422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -436,7 +436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -450,7 +450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -464,7 +464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -478,7 +478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2021</v>
       </c>
@@ -492,7 +492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2021</v>
       </c>
@@ -506,7 +506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2021</v>
       </c>
@@ -520,7 +520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -534,7 +534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -548,7 +548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -562,7 +562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -576,7 +576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2021</v>
       </c>
@@ -590,7 +590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -604,7 +604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2021</v>
       </c>
@@ -618,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2021</v>
       </c>
@@ -632,7 +632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2021</v>
       </c>
@@ -646,7 +646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2021</v>
       </c>
@@ -660,7 +660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2022</v>
       </c>
@@ -674,7 +674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2022</v>
       </c>
@@ -688,7 +688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2022</v>
       </c>
@@ -702,7 +702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2022</v>
       </c>
@@ -716,7 +716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2022</v>
       </c>
@@ -730,7 +730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2022</v>
       </c>
@@ -744,7 +744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2022</v>
       </c>
@@ -758,7 +758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2022</v>
       </c>
@@ -772,7 +772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2022</v>
       </c>
@@ -786,7 +786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2022</v>
       </c>
@@ -800,7 +800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2022</v>
       </c>
@@ -814,7 +814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2022</v>
       </c>
@@ -828,7 +828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2022</v>
       </c>
@@ -845,7 +845,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2022</v>
       </c>
@@ -862,7 +862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2022</v>
       </c>
@@ -879,7 +879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2022</v>
       </c>
@@ -896,7 +896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2022</v>
       </c>
@@ -910,7 +910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2022</v>
       </c>
@@ -924,7 +924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2022</v>
       </c>
@@ -938,7 +938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2022</v>
       </c>
@@ -952,7 +952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2022</v>
       </c>
@@ -969,7 +969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2022</v>
       </c>
@@ -983,7 +983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2022</v>
       </c>
@@ -997,7 +997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2023</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2023</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2023</v>
       </c>
@@ -1036,6 +1036,20 @@
         <v>7</v>
       </c>
       <c r="E45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2023</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first pass of visit 10 data
</commit_message>
<xml_diff>
--- a/data/visit_dates.xlsx
+++ b/data/visit_dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/r_repositories/rodent_trapping/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucbtds4\R_Repositories\rodent_trapping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F24920-CBB7-9246-904C-35D9A0395EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8F54A1-90B5-414A-A6F7-5954AEA77AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -383,15 +383,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -422,7 +422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -436,7 +436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -450,7 +450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -464,7 +464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -478,7 +478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2021</v>
       </c>
@@ -492,7 +492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2021</v>
       </c>
@@ -506,7 +506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2021</v>
       </c>
@@ -520,7 +520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -534,7 +534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -548,7 +548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -562,7 +562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -576,7 +576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2021</v>
       </c>
@@ -590,7 +590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -604,7 +604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2021</v>
       </c>
@@ -618,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2021</v>
       </c>
@@ -632,7 +632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2021</v>
       </c>
@@ -646,7 +646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2021</v>
       </c>
@@ -660,7 +660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2022</v>
       </c>
@@ -674,7 +674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2022</v>
       </c>
@@ -688,7 +688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2022</v>
       </c>
@@ -702,7 +702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2022</v>
       </c>
@@ -716,7 +716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2022</v>
       </c>
@@ -730,7 +730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2022</v>
       </c>
@@ -744,7 +744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2022</v>
       </c>
@@ -758,7 +758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2022</v>
       </c>
@@ -772,7 +772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2022</v>
       </c>
@@ -786,7 +786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2022</v>
       </c>
@@ -800,7 +800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2022</v>
       </c>
@@ -814,7 +814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2022</v>
       </c>
@@ -828,7 +828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2022</v>
       </c>
@@ -845,7 +845,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2022</v>
       </c>
@@ -862,7 +862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2022</v>
       </c>
@@ -879,7 +879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2022</v>
       </c>
@@ -896,7 +896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2022</v>
       </c>
@@ -910,7 +910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2022</v>
       </c>
@@ -924,7 +924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2022</v>
       </c>
@@ -938,7 +938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2022</v>
       </c>
@@ -952,7 +952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2022</v>
       </c>
@@ -969,7 +969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2022</v>
       </c>
@@ -983,7 +983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2022</v>
       </c>
@@ -997,7 +997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2023</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2023</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2023</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2023</v>
       </c>
@@ -1051,6 +1051,104 @@
       </c>
       <c r="E46">
         <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2023</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2023</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2023</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2023</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2023</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2023</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>2023</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>